<commit_message>
Added call back to events
</commit_message>
<xml_diff>
--- a/build/ccd-development-config/ccd-prl-dev.xlsx
+++ b/build/ccd-development-config/ccd-prl-dev.xlsx
@@ -43953,7 +43953,9 @@
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
-      <c r="N9"/>
+      <c r="N9" t="s">
+        <v>815</v>
+      </c>
       <c r="O9"/>
       <c r="P9" t="s">
         <v>232</v>
@@ -44045,7 +44047,9 @@
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
-      <c r="N11"/>
+      <c r="N11" t="s">
+        <v>815</v>
+      </c>
       <c r="O11"/>
       <c r="P11" t="s">
         <v>232</v>
@@ -44137,7 +44141,9 @@
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13"/>
+      <c r="N13" t="s">
+        <v>815</v>
+      </c>
       <c r="O13"/>
       <c r="P13" t="s">
         <v>232</v>
@@ -44183,7 +44189,9 @@
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14"/>
+      <c r="N14" t="s">
+        <v>815</v>
+      </c>
       <c r="O14"/>
       <c r="P14" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Added call back url for task list to additional events
</commit_message>
<xml_diff>
--- a/build/ccd-development-config/ccd-prl-dev.xlsx
+++ b/build/ccd-development-config/ccd-prl-dev.xlsx
@@ -44375,7 +44375,9 @@
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18"/>
+      <c r="N18" t="s">
+        <v>815</v>
+      </c>
       <c r="O18"/>
       <c r="P18" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
added call backs to more events
</commit_message>
<xml_diff>
--- a/build/ccd-development-config/ccd-prl-dev.xlsx
+++ b/build/ccd-development-config/ccd-prl-dev.xlsx
@@ -43861,7 +43861,9 @@
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
-      <c r="N7"/>
+      <c r="N7" t="s">
+        <v>815</v>
+      </c>
       <c r="O7"/>
       <c r="P7" t="s">
         <v>232</v>
@@ -43907,7 +43909,9 @@
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
-      <c r="N8"/>
+      <c r="N8" t="s">
+        <v>815</v>
+      </c>
       <c r="O8"/>
       <c r="P8" t="s">
         <v>232</v>
@@ -44237,7 +44241,9 @@
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15"/>
+      <c r="N15" t="s">
+        <v>815</v>
+      </c>
       <c r="O15"/>
       <c r="P15" t="s">
         <v>232</v>
@@ -44283,7 +44289,9 @@
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
-      <c r="N16"/>
+      <c r="N16" t="s">
+        <v>815</v>
+      </c>
       <c r="O16"/>
       <c r="P16" t="s">
         <v>232</v>
@@ -44329,7 +44337,9 @@
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17"/>
+      <c r="N17" t="s">
+        <v>815</v>
+      </c>
       <c r="O17"/>
       <c r="P17" t="s">
         <v>232</v>
@@ -44423,7 +44433,9 @@
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
-      <c r="N19"/>
+      <c r="N19" t="s">
+        <v>815</v>
+      </c>
       <c r="O19"/>
       <c r="P19" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
Remove the EventElementLabel = null
</commit_message>
<xml_diff>
--- a/build/ccd-development-config/ccd-prl-dev.xlsx
+++ b/build/ccd-development-config/ccd-prl-dev.xlsx
@@ -1476,7 +1476,7 @@
     <t xml:space="preserve">PartyDetails</t>
   </si>
   <si>
-    <t xml:space="preserve">textApplicants</t>
+    <t xml:space="preserve">typeOfApplication</t>
   </si>
   <si>
     <t xml:space="preserve">applicantsFL401</t>
@@ -2566,10 +2566,10 @@
     <t xml:space="preserve">applicantsDetails</t>
   </si>
   <si>
-    <t xml:space="preserve">textApplicants="C100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">textApplicants="FL401"</t>
+    <t xml:space="preserve">typeOfApplication="C100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">typeOfApplication="FL401"</t>
   </si>
   <si>
     <t xml:space="preserve">applicantsFL401="DO_NOT_SHOW"</t>
@@ -33250,10 +33250,10 @@
         <v>448</v>
       </c>
       <c r="E1136" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="F1136" t="s">
-        <v>1448</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1137">
@@ -33265,7 +33265,7 @@
         <v>227</v>
       </c>
       <c r="D1137" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E1137" t="s">
         <v>1449</v>
@@ -33283,10 +33283,10 @@
         <v>227</v>
       </c>
       <c r="D1138" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E1138" t="s">
-        <v>1447</v>
+        <v>1450</v>
       </c>
       <c r="F1138" t="s">
         <v>1455</v>
@@ -33301,13 +33301,13 @@
         <v>227</v>
       </c>
       <c r="D1139" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E1139" t="s">
-        <v>1449</v>
+        <v>1452</v>
       </c>
       <c r="F1139" t="s">
-        <v>1448</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1140">
@@ -33319,10 +33319,10 @@
         <v>227</v>
       </c>
       <c r="D1140" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E1140" t="s">
-        <v>1450</v>
+        <v>1453</v>
       </c>
       <c r="F1140" t="s">
         <v>1455</v>
@@ -33337,10 +33337,10 @@
         <v>227</v>
       </c>
       <c r="D1141" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="E1141" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="F1141" t="s">
         <v>1455</v>
@@ -33355,12 +33355,156 @@
         <v>227</v>
       </c>
       <c r="D1142" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1142" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F1142" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1143" s="1"/>
+      <c r="C1143" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1143" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1143" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F1143" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1144" s="1"/>
+      <c r="C1144" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1144" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1144" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F1144" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1145" s="1"/>
+      <c r="C1145" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1145" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1145" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F1145" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1146" s="1"/>
+      <c r="C1146" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1146" t="s">
         <v>453</v>
       </c>
-      <c r="E1142" t="s">
+      <c r="E1146" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F1146" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1147" s="1"/>
+      <c r="C1147" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1147" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1147" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F1147" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1148" s="1"/>
+      <c r="C1148" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1148" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1148" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F1148" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1149" s="1"/>
+      <c r="C1149" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1149" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1149" t="s">
+        <v>1452</v>
+      </c>
+      <c r="F1149" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B1150" s="1"/>
+      <c r="C1150" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1150" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1150" t="s">
         <v>1453</v>
       </c>
-      <c r="F1142" t="s">
+      <c r="F1150" t="s">
         <v>1455</v>
       </c>
     </row>

</xml_diff>